<commit_message>
Ajustes importaciones, materia prima
</commit_message>
<xml_diff>
--- a/cost/assets/formatsXlsx/Materia_prima.xlsx
+++ b/cost/assets/formatsXlsx/Materia_prima.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\apps\htdocs\tezlikv2\app\assets\formatsXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Ledesma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662C25BD-99BD-407E-8A7D-E55CDA25BB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DDB233-2868-42B4-8B1F-E1F537CFBF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -248,49 +248,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Roboto"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Roboto"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -399,10 +356,53 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -419,12 +419,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="referencia" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="material" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="unidad" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="costo" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="referencia" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="material" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="unidad" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="costo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -753,9 +753,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" style="3" customWidth="1"/>
@@ -763,7 +765,7 @@
     <col min="5" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,49 +779,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="1"/>
       <c r="C3" s="8"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="1"/>
       <c r="C4" s="8"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="1"/>
       <c r="C5" s="8"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="1"/>
       <c r="C6" s="8"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>

</xml_diff>